<commit_message>
Jenkins refactored; Added Additonal Features with related java classes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/Scotiabank_Data.xlsx
+++ b/src/test/resources/testData/Scotiabank_Data.xlsx
@@ -3,17 +3,24 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29231"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B3AF2219-06D1-4529-95A5-F9F9AFEAA98C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\ECLIPSE_PLAYGROUND\ScotiaBankAutomationProject\src\test\resources\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C5A24C1-9785-409D-8B71-FBDFEBE81E62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Config" sheetId="1" r:id="rId1"/>
     <sheet name="CC_DetailedSpend" sheetId="2" r:id="rId2"/>
     <sheet name="CC_AverageSpend" sheetId="3" r:id="rId3"/>
+    <sheet name="TFSA" sheetId="4" r:id="rId4"/>
+    <sheet name="AutoLoanCalculator" sheetId="5" r:id="rId5"/>
+    <sheet name="MortgageLoanCalculator" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:Q34"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
   <si>
     <t>key</t>
   </si>
@@ -43,9 +50,6 @@
     <t>ccRewardCalcUrl</t>
   </si>
   <si>
-    <t>https://www.scotiabank.com/</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.scotiabank.com/ca/en/personal/credit-cards/scene-points-rewards-calculator.html#/ </t>
   </si>
   <si>
@@ -74,13 +78,70 @@
   </si>
   <si>
     <t>spend</t>
+  </si>
+  <si>
+    <t>Years</t>
+  </si>
+  <si>
+    <t>StartingAmount</t>
+  </si>
+  <si>
+    <t>PeriodicInvestment</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>AnnualIncome</t>
+  </si>
+  <si>
+    <t>Monthly</t>
+  </si>
+  <si>
+    <t>ON</t>
+  </si>
+  <si>
+    <t>BC</t>
+  </si>
+  <si>
+    <t>tfsaUrl</t>
+  </si>
+  <si>
+    <t>https://www.scotiabank.com/ca/en/personal/investing/tax-free-savings-account/tfsa-calculator.html</t>
+  </si>
+  <si>
+    <t>https://www.scotiabank.com/ca/en/personal.html</t>
+  </si>
+  <si>
+    <t>MortgageAmount</t>
+  </si>
+  <si>
+    <t>AmortizationPeriod</t>
+  </si>
+  <si>
+    <t>InterestRate</t>
+  </si>
+  <si>
+    <t>loan</t>
+  </si>
+  <si>
+    <t>DownPayment</t>
+  </si>
+  <si>
+    <t>Months</t>
+  </si>
+  <si>
+    <t>IntRate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +160,12 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Consolas"/>
       <family val="3"/>
     </font>
@@ -124,11 +191,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -410,16 +483,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="87.7109375" customWidth="1"/>
+    <col min="2" max="2" width="93.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -443,7 +516,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -451,13 +524,22 @@
         <v>5</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" xr:uid="{BD4A979A-39F5-4141-BB61-2CFDE182A256}"/>
     <hyperlink ref="B4" r:id="rId2" location="/ " xr:uid="{98CB9F22-7054-4FB4-BFD0-08B1D12945C1}"/>
+    <hyperlink ref="B5" r:id="rId3" xr:uid="{2F660E32-F1C5-467C-852F-5A4115BD4261}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -482,28 +564,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -749,7 +831,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{318E8A5D-D9F1-4B43-BAA5-337CEB197354}">
   <dimension ref="A1:A9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -757,7 +839,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -798,6 +880,363 @@
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>1234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EC8BE9-6416-48AF-AA26-58DC484FDBF5}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="6" max="6" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="4">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C2" s="4">
+        <v>100</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="4">
+        <v>50000</v>
+      </c>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="4">
+        <v>15</v>
+      </c>
+      <c r="B3" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C3" s="4">
+        <v>200</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F3" s="4">
+        <v>75000</v>
+      </c>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="4">
+        <v>10</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="4">
+        <v>100</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="4">
+        <v>15</v>
+      </c>
+      <c r="B5" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C5" s="4">
+        <v>200</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4">
+        <v>10</v>
+      </c>
+      <c r="B6" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C6" s="4">
+        <v>100</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="4">
+        <v>15</v>
+      </c>
+      <c r="B7" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C7" s="4">
+        <v>200</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="4">
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="4">
+        <v>10</v>
+      </c>
+      <c r="B8" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C8" s="4">
+        <v>100</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="4">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>15</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C9" s="4">
+        <v>200</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F9" s="4">
+        <v>75000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BBF123-9D61-4099-A0EC-96B208E5AAFE}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <v>25000</v>
+      </c>
+      <c r="B2" s="6">
+        <v>100</v>
+      </c>
+      <c r="C2" s="6">
+        <v>96</v>
+      </c>
+      <c r="D2" s="6">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>30000</v>
+      </c>
+      <c r="B3" s="6">
+        <v>1000</v>
+      </c>
+      <c r="C3" s="6">
+        <v>48</v>
+      </c>
+      <c r="D3" s="6">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>35000</v>
+      </c>
+      <c r="B4" s="6">
+        <v>5000</v>
+      </c>
+      <c r="C4" s="6">
+        <v>72</v>
+      </c>
+      <c r="D4" s="6">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>80000</v>
+      </c>
+      <c r="B5" s="6">
+        <v>15000</v>
+      </c>
+      <c r="C5" s="6">
+        <v>96</v>
+      </c>
+      <c r="D5" s="6">
+        <v>7.49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93A81B98-2D7D-4012-91FC-57CA44A79EED}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>400000</v>
+      </c>
+      <c r="B2" s="5">
+        <v>20</v>
+      </c>
+      <c r="C2" s="5">
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>550000</v>
+      </c>
+      <c r="B3" s="5">
+        <v>25</v>
+      </c>
+      <c r="C3" s="5">
+        <v>4.99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>750000</v>
+      </c>
+      <c r="B4" s="5">
+        <v>30</v>
+      </c>
+      <c r="C4" s="5">
+        <v>5.49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>